<commit_message>
added parser and updated agents to reset between games
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Foos\repos\mtree_cooperation_tournament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B7AC80-F819-4969-8D9C-51ED6D97F263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BFE37A-4A4F-47D4-804E-AA2891363CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="1845" windowWidth="21600" windowHeight="11385" xr2:uid="{7FAD7775-8CEE-4477-8DE6-83B43C94E46D}"/>
+    <workbookView xWindow="7335" yWindow="3585" windowWidth="21600" windowHeight="11385" xr2:uid="{7FAD7775-8CEE-4477-8DE6-83B43C94E46D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD32C77-04C8-49AF-86BF-412060158E0C}">
-  <dimension ref="A4:K33"/>
+  <dimension ref="A4:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,20 +598,94 @@
         <v>679</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C18" t="str">
+        <f>B19</f>
+        <v>Tit for Tat</v>
+      </c>
+      <c r="D18" t="str">
+        <f>B20</f>
+        <v>Tideman</v>
+      </c>
+      <c r="E18" t="str">
+        <f>B21</f>
+        <v>Nydegger</v>
+      </c>
+      <c r="F18" t="str">
+        <f>B22</f>
+        <v>Grofman</v>
+      </c>
+      <c r="G18" t="str">
+        <f>B23</f>
+        <v>Shubik</v>
+      </c>
+      <c r="H18" t="str">
+        <f>B24</f>
+        <v>Stein</v>
+      </c>
+      <c r="I18" t="str">
+        <f>B25</f>
+        <v>Friedman</v>
+      </c>
+      <c r="J18" t="str">
+        <f>B26</f>
+        <v>Davis</v>
+      </c>
+      <c r="K18" t="str">
+        <f>B27</f>
+        <v>Graaskamp</v>
+      </c>
+      <c r="L18" t="str">
+        <f>B28</f>
+        <v>Downing</v>
+      </c>
+      <c r="M18" t="str">
+        <f>B29</f>
+        <v>Feld</v>
+      </c>
+      <c r="N18" t="str">
+        <f>B30</f>
+        <v>Joss</v>
+      </c>
+      <c r="O18" t="str">
+        <f>B31</f>
+        <v>Tullock</v>
+      </c>
+      <c r="P18" t="str">
+        <f>B32</f>
+        <v>(no name)</v>
+      </c>
+      <c r="Q18" t="str">
+        <f>B33</f>
+        <v>Random</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>600</v>
+      </c>
+      <c r="M19">
+        <v>283</v>
+      </c>
+      <c r="N19">
+        <v>283</v>
+      </c>
+      <c r="Q19">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -619,15 +693,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>600</v>
+      </c>
+      <c r="M21">
+        <v>429</v>
+      </c>
+      <c r="N21">
+        <v>564</v>
+      </c>
+      <c r="Q21">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -635,7 +721,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -643,7 +729,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -651,12 +737,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -664,7 +750,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -672,7 +758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -680,23 +766,47 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>288</v>
+      </c>
+      <c r="E29">
+        <v>714</v>
+      </c>
+      <c r="N29">
+        <v>286</v>
+      </c>
+      <c r="Q29">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>288</v>
+      </c>
+      <c r="E30">
+        <v>624</v>
+      </c>
+      <c r="M30">
+        <v>286</v>
+      </c>
+      <c r="Q30">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -704,7 +814,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -712,12 +822,24 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>20</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
+      </c>
+      <c r="C33">
+        <v>441</v>
+      </c>
+      <c r="E33">
+        <v>774</v>
+      </c>
+      <c r="M33">
+        <v>373</v>
+      </c>
+      <c r="N33">
+        <v>415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>